<commit_message>
Updated subclade exon trees
</commit_message>
<xml_diff>
--- a/tabular/refseq-lineage/ifnl-curated-side-data-mammalia.xlsx
+++ b/tabular/refseq-lineage/ifnl-curated-side-data-mammalia.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11211"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/host/IFNL-GLUE/tabular/refseq-lineage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92114479-6128-2E46-A601-B323F7D00339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E8319F-1E41-184E-98A1-C96953F851FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7820" yWindow="6060" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A+B" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2576" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2936" uniqueCount="635">
   <si>
     <t>retroIFNL1a</t>
   </si>
@@ -1747,6 +1748,198 @@
   </si>
   <si>
     <t>Rhinopithecus bieti</t>
+  </si>
+  <si>
+    <t>NM_001142837</t>
+  </si>
+  <si>
+    <t>NW_016529666</t>
+  </si>
+  <si>
+    <t>XM_011973358</t>
+  </si>
+  <si>
+    <t>XM_012775211</t>
+  </si>
+  <si>
+    <t>XM_015820664</t>
+  </si>
+  <si>
+    <t>XM_029924289</t>
+  </si>
+  <si>
+    <t>XM_030796492</t>
+  </si>
+  <si>
+    <t>XM_032273584</t>
+  </si>
+  <si>
+    <t>XM_032326013</t>
+  </si>
+  <si>
+    <t>XM_032850864</t>
+  </si>
+  <si>
+    <t>XM_033226159</t>
+  </si>
+  <si>
+    <t>XM_008173201</t>
+  </si>
+  <si>
+    <t>Protobothrops mucrosquamatus</t>
+  </si>
+  <si>
+    <t>Gorilla gorilla gorilla</t>
+  </si>
+  <si>
+    <t>Suricata suricatta</t>
+  </si>
+  <si>
+    <t>Sapajus apella</t>
+  </si>
+  <si>
+    <t>Mustela erminea</t>
+  </si>
+  <si>
+    <t>Lontra canadensis</t>
+  </si>
+  <si>
+    <t>Trachypithecus francoisi</t>
+  </si>
+  <si>
+    <t>Chrysemys picta bellii</t>
+  </si>
+  <si>
+    <t>Mandrillus</t>
+  </si>
+  <si>
+    <t>Cheirogaleidae</t>
+  </si>
+  <si>
+    <t>Microcebus</t>
+  </si>
+  <si>
+    <t>Lepidosauria</t>
+  </si>
+  <si>
+    <t>Squamata</t>
+  </si>
+  <si>
+    <t>Viperidae</t>
+  </si>
+  <si>
+    <t>Protobothrops</t>
+  </si>
+  <si>
+    <t>Rhinopithecus</t>
+  </si>
+  <si>
+    <t>Piliocolobus</t>
+  </si>
+  <si>
+    <t>Pongo</t>
+  </si>
+  <si>
+    <t>Theropithecus</t>
+  </si>
+  <si>
+    <t>Herpestidae</t>
+  </si>
+  <si>
+    <t>Suricata</t>
+  </si>
+  <si>
+    <t>Sapajus</t>
+  </si>
+  <si>
+    <t>Mustela</t>
+  </si>
+  <si>
+    <t>Lontra</t>
+  </si>
+  <si>
+    <t>Trachypithecus</t>
+  </si>
+  <si>
+    <t>Testudines</t>
+  </si>
+  <si>
+    <t>Emydidae</t>
+  </si>
+  <si>
+    <t>Chrysemys</t>
+  </si>
+  <si>
+    <t>Saimiri</t>
+  </si>
+  <si>
+    <t>Aotidae</t>
+  </si>
+  <si>
+    <t>Aotus</t>
+  </si>
+  <si>
+    <t>Cercocebus</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-3</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-4</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-5</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-6</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-7</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-8</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-9</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-10</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-11</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-12</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-13</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-14</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-15</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-16</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-17</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-18</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-19</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-20</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-21</t>
+  </si>
+  <si>
+    <t>IFNL-B-Mammal-22</t>
   </si>
 </sst>
 </file>
@@ -3375,10 +3568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R222"/>
+  <dimension ref="A1:R241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="F23" sqref="A1:R222"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="C239" sqref="A1:R241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12092,13 +12285,27 @@
         <v>308</v>
       </c>
       <c r="H188" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I188" s="11"/>
-      <c r="J188" s="17"/>
+      <c r="J188" s="7"/>
       <c r="K188" s="11">
         <v>2</v>
       </c>
+      <c r="L188" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M188" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N188" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O188" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="P188" s="7"/>
+      <c r="Q188" s="7"/>
       <c r="R188" s="7"/>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.2">
@@ -12124,13 +12331,27 @@
         <v>308</v>
       </c>
       <c r="H189" s="11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I189" s="11"/>
       <c r="J189" s="7"/>
       <c r="K189" s="11">
         <v>2</v>
       </c>
+      <c r="L189" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M189" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N189" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O189" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P189" s="7"/>
+      <c r="Q189" s="7"/>
       <c r="R189" s="7"/>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.2">
@@ -12156,13 +12377,27 @@
         <v>308</v>
       </c>
       <c r="H190" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I190" s="11"/>
       <c r="J190" s="7"/>
       <c r="K190" s="11">
         <v>2</v>
       </c>
+      <c r="L190" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M190" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N190" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="O190" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="P190" s="7"/>
+      <c r="Q190" s="7"/>
       <c r="R190" s="7"/>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.2">
@@ -12188,13 +12423,27 @@
         <v>308</v>
       </c>
       <c r="H191" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I191" s="11"/>
-      <c r="J191" s="17"/>
+      <c r="J191" s="7"/>
       <c r="K191" s="11">
         <v>2</v>
       </c>
+      <c r="L191" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M191" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N191" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O191" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="P191" s="7"/>
+      <c r="Q191" s="7"/>
       <c r="R191" s="7"/>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.2">
@@ -12220,13 +12469,27 @@
         <v>308</v>
       </c>
       <c r="H192" s="11">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I192" s="11"/>
       <c r="J192" s="7"/>
       <c r="K192" s="11">
         <v>2</v>
       </c>
+      <c r="L192" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M192" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N192" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="O192" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="P192" s="7"/>
+      <c r="Q192" s="7"/>
       <c r="R192" s="7"/>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.2">
@@ -12252,13 +12515,27 @@
         <v>308</v>
       </c>
       <c r="H193" s="11">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I193" s="11"/>
       <c r="J193" s="7"/>
       <c r="K193" s="11">
         <v>2</v>
       </c>
+      <c r="L193" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M193" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N193" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O193" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="P193" s="7"/>
+      <c r="Q193" s="7"/>
       <c r="R193" s="7"/>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
@@ -12284,13 +12561,27 @@
         <v>308</v>
       </c>
       <c r="H194" s="11">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I194" s="11"/>
-      <c r="J194" s="17"/>
+      <c r="J194" s="7"/>
       <c r="K194" s="11">
         <v>2</v>
       </c>
+      <c r="L194" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M194" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N194" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O194" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="P194" s="7"/>
+      <c r="Q194" s="7"/>
       <c r="R194" s="7"/>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.2">
@@ -12316,13 +12607,27 @@
         <v>308</v>
       </c>
       <c r="H195" s="11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I195" s="11"/>
       <c r="J195" s="7"/>
       <c r="K195" s="11">
         <v>2</v>
       </c>
+      <c r="L195" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M195" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N195" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O195" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="P195" s="7"/>
+      <c r="Q195" s="7"/>
       <c r="R195" s="7"/>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.2">
@@ -12348,13 +12653,27 @@
         <v>308</v>
       </c>
       <c r="H196" s="11">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I196" s="11"/>
       <c r="J196" s="7"/>
       <c r="K196" s="11">
         <v>2</v>
       </c>
+      <c r="L196" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M196" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N196" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O196" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="P196" s="7"/>
+      <c r="Q196" s="7"/>
       <c r="R196" s="7"/>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.2">
@@ -12380,13 +12699,27 @@
         <v>308</v>
       </c>
       <c r="H197" s="11">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I197" s="11"/>
-      <c r="J197" s="17"/>
+      <c r="J197" s="7"/>
       <c r="K197" s="11">
         <v>2</v>
       </c>
+      <c r="L197" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M197" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N197" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O197" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="P197" s="7"/>
+      <c r="Q197" s="7"/>
       <c r="R197" s="7"/>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
@@ -12412,13 +12745,27 @@
         <v>308</v>
       </c>
       <c r="H198" s="11">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="I198" s="11"/>
       <c r="J198" s="7"/>
       <c r="K198" s="11">
         <v>2</v>
       </c>
+      <c r="L198" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M198" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N198" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O198" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="P198" s="7"/>
+      <c r="Q198" s="7"/>
       <c r="R198" s="7"/>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
@@ -12444,13 +12791,27 @@
         <v>308</v>
       </c>
       <c r="H199" s="11">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="I199" s="11"/>
       <c r="J199" s="7"/>
       <c r="K199" s="11">
         <v>2</v>
       </c>
+      <c r="L199" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M199" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N199" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O199" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="P199" s="7"/>
+      <c r="Q199" s="7"/>
       <c r="R199" s="7"/>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
@@ -12476,13 +12837,27 @@
         <v>308</v>
       </c>
       <c r="H200" s="11">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="I200" s="11"/>
-      <c r="J200" s="17"/>
+      <c r="J200" s="7"/>
       <c r="K200" s="11">
         <v>2</v>
       </c>
+      <c r="L200" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M200" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N200" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O200" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P200" s="7"/>
+      <c r="Q200" s="7"/>
       <c r="R200" s="7"/>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.2">
@@ -12508,13 +12883,27 @@
         <v>308</v>
       </c>
       <c r="H201" s="11">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="I201" s="11"/>
       <c r="J201" s="7"/>
       <c r="K201" s="11">
         <v>2</v>
       </c>
+      <c r="L201" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M201" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N201" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O201" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P201" s="7"/>
+      <c r="Q201" s="7"/>
       <c r="R201" s="7"/>
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.2">
@@ -12540,13 +12929,27 @@
         <v>308</v>
       </c>
       <c r="H202" s="11">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I202" s="11"/>
       <c r="J202" s="7"/>
       <c r="K202" s="11">
         <v>2</v>
       </c>
+      <c r="L202" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M202" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N202" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O202" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P202" s="7"/>
+      <c r="Q202" s="7"/>
       <c r="R202" s="7"/>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.2">
@@ -12572,13 +12975,27 @@
         <v>308</v>
       </c>
       <c r="H203" s="11">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="I203" s="11"/>
-      <c r="J203" s="17"/>
+      <c r="J203" s="7"/>
       <c r="K203" s="11">
         <v>2</v>
       </c>
+      <c r="L203" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M203" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N203" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O203" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="P203" s="7"/>
+      <c r="Q203" s="7"/>
       <c r="R203" s="7"/>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.2">
@@ -12604,13 +13021,27 @@
         <v>308</v>
       </c>
       <c r="H204" s="11">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="I204" s="11"/>
       <c r="J204" s="7"/>
       <c r="K204" s="11">
         <v>2</v>
       </c>
+      <c r="L204" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M204" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N204" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O204" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="P204" s="7"/>
+      <c r="Q204" s="7"/>
       <c r="R204" s="7"/>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.2">
@@ -12636,13 +13067,27 @@
         <v>308</v>
       </c>
       <c r="H205" s="11">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="I205" s="11"/>
       <c r="J205" s="7"/>
       <c r="K205" s="11">
         <v>2</v>
       </c>
+      <c r="L205" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M205" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N205" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O205" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="P205" s="7"/>
+      <c r="Q205" s="7"/>
       <c r="R205" s="7"/>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.2">
@@ -12668,13 +13113,27 @@
         <v>308</v>
       </c>
       <c r="H206" s="11">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="I206" s="11"/>
-      <c r="J206" s="17"/>
+      <c r="J206" s="7"/>
       <c r="K206" s="11">
         <v>2</v>
       </c>
+      <c r="L206" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M206" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N206" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O206" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="P206" s="7"/>
+      <c r="Q206" s="7"/>
       <c r="R206" s="7"/>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.2">
@@ -12700,13 +13159,27 @@
         <v>308</v>
       </c>
       <c r="H207" s="11">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I207" s="11"/>
       <c r="J207" s="7"/>
       <c r="K207" s="11">
         <v>2</v>
       </c>
+      <c r="L207" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M207" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N207" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="O207" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="P207" s="7"/>
+      <c r="Q207" s="7"/>
       <c r="R207" s="7"/>
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.2">
@@ -12732,13 +13205,27 @@
         <v>308</v>
       </c>
       <c r="H208" s="11">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="I208" s="11"/>
       <c r="J208" s="7"/>
       <c r="K208" s="11">
         <v>2</v>
       </c>
+      <c r="L208" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M208" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N208" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O208" s="7" t="s">
+        <v>611</v>
+      </c>
+      <c r="P208" s="7"/>
+      <c r="Q208" s="7"/>
       <c r="R208" s="7"/>
     </row>
     <row r="209" spans="1:18" x14ac:dyDescent="0.2">
@@ -12764,13 +13251,27 @@
         <v>308</v>
       </c>
       <c r="H209" s="11">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="I209" s="11"/>
-      <c r="J209" s="17"/>
+      <c r="J209" s="7"/>
       <c r="K209" s="11">
         <v>2</v>
       </c>
+      <c r="L209" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M209" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N209" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="O209" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="P209" s="7"/>
+      <c r="Q209" s="7"/>
       <c r="R209" s="7"/>
     </row>
     <row r="210" spans="1:18" x14ac:dyDescent="0.2">
@@ -12796,13 +13297,27 @@
         <v>308</v>
       </c>
       <c r="H210" s="11">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="I210" s="11"/>
       <c r="J210" s="7"/>
       <c r="K210" s="11">
         <v>2</v>
       </c>
+      <c r="L210" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M210" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N210" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O210" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="P210" s="7"/>
+      <c r="Q210" s="7"/>
       <c r="R210" s="7"/>
     </row>
     <row r="211" spans="1:18" x14ac:dyDescent="0.2">
@@ -12828,13 +13343,27 @@
         <v>308</v>
       </c>
       <c r="H211" s="11">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="I211" s="11"/>
       <c r="J211" s="7"/>
       <c r="K211" s="11">
         <v>2</v>
       </c>
+      <c r="L211" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M211" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N211" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O211" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="P211" s="7"/>
+      <c r="Q211" s="7"/>
       <c r="R211" s="7"/>
     </row>
     <row r="212" spans="1:18" x14ac:dyDescent="0.2">
@@ -12860,13 +13389,27 @@
         <v>308</v>
       </c>
       <c r="H212" s="11">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="I212" s="11"/>
-      <c r="J212" s="17"/>
+      <c r="J212" s="7"/>
       <c r="K212" s="11">
         <v>2</v>
       </c>
+      <c r="L212" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M212" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N212" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O212" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="P212" s="7"/>
+      <c r="Q212" s="7"/>
       <c r="R212" s="7"/>
     </row>
     <row r="213" spans="1:18" x14ac:dyDescent="0.2">
@@ -12892,13 +13435,27 @@
         <v>308</v>
       </c>
       <c r="H213" s="11">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="I213" s="11"/>
       <c r="J213" s="7"/>
       <c r="K213" s="11">
         <v>2</v>
       </c>
+      <c r="L213" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M213" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N213" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O213" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="P213" s="7"/>
+      <c r="Q213" s="7"/>
       <c r="R213" s="7"/>
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.2">
@@ -12924,13 +13481,27 @@
         <v>308</v>
       </c>
       <c r="H214" s="11">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="I214" s="11"/>
       <c r="J214" s="7"/>
       <c r="K214" s="11">
         <v>2</v>
       </c>
+      <c r="L214" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M214" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N214" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O214" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="P214" s="7"/>
+      <c r="Q214" s="7"/>
       <c r="R214" s="7"/>
     </row>
     <row r="215" spans="1:18" x14ac:dyDescent="0.2">
@@ -12956,13 +13527,27 @@
         <v>308</v>
       </c>
       <c r="H215" s="11">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="I215" s="11"/>
-      <c r="J215" s="17"/>
+      <c r="J215" s="7"/>
       <c r="K215" s="11">
         <v>2</v>
       </c>
+      <c r="L215" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M215" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N215" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O215" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="P215" s="7"/>
+      <c r="Q215" s="7"/>
       <c r="R215" s="7"/>
     </row>
     <row r="216" spans="1:18" x14ac:dyDescent="0.2">
@@ -12988,13 +13573,27 @@
         <v>308</v>
       </c>
       <c r="H216" s="11">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="I216" s="11"/>
       <c r="J216" s="7"/>
       <c r="K216" s="11">
         <v>2</v>
       </c>
+      <c r="L216" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M216" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N216" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O216" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P216" s="7"/>
+      <c r="Q216" s="7"/>
       <c r="R216" s="7"/>
     </row>
     <row r="217" spans="1:18" x14ac:dyDescent="0.2">
@@ -13020,13 +13619,27 @@
         <v>308</v>
       </c>
       <c r="H217" s="11">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="I217" s="11"/>
       <c r="J217" s="7"/>
       <c r="K217" s="11">
         <v>2</v>
       </c>
+      <c r="L217" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M217" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N217" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O217" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="P217" s="7"/>
+      <c r="Q217" s="7"/>
       <c r="R217" s="7"/>
     </row>
     <row r="218" spans="1:18" x14ac:dyDescent="0.2">
@@ -13052,13 +13665,27 @@
         <v>308</v>
       </c>
       <c r="H218" s="11">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="I218" s="11"/>
-      <c r="J218" s="17"/>
+      <c r="J218" s="7"/>
       <c r="K218" s="11">
         <v>2</v>
       </c>
+      <c r="L218" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M218" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N218" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O218" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="P218" s="7"/>
+      <c r="Q218" s="7"/>
       <c r="R218" s="7"/>
     </row>
     <row r="219" spans="1:18" x14ac:dyDescent="0.2">
@@ -13084,13 +13711,27 @@
         <v>308</v>
       </c>
       <c r="H219" s="11">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="I219" s="11"/>
       <c r="J219" s="7"/>
       <c r="K219" s="11">
         <v>2</v>
       </c>
+      <c r="L219" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M219" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N219" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O219" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="P219" s="7"/>
+      <c r="Q219" s="7"/>
       <c r="R219" s="7"/>
     </row>
     <row r="220" spans="1:18" x14ac:dyDescent="0.2">
@@ -13116,13 +13757,27 @@
         <v>308</v>
       </c>
       <c r="H220" s="11">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="I220" s="11"/>
       <c r="J220" s="7"/>
       <c r="K220" s="11">
         <v>2</v>
       </c>
+      <c r="L220" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M220" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N220" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O220" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="P220" s="7"/>
+      <c r="Q220" s="7"/>
       <c r="R220" s="7"/>
     </row>
     <row r="221" spans="1:18" x14ac:dyDescent="0.2">
@@ -13148,13 +13803,27 @@
         <v>308</v>
       </c>
       <c r="H221" s="11">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="I221" s="11"/>
-      <c r="J221" s="17"/>
+      <c r="J221" s="7"/>
       <c r="K221" s="11">
         <v>2</v>
       </c>
+      <c r="L221" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M221" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N221" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="O221" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="P221" s="7"/>
+      <c r="Q221" s="7"/>
       <c r="R221" s="7"/>
     </row>
     <row r="222" spans="1:18" x14ac:dyDescent="0.2">
@@ -13180,14 +13849,902 @@
         <v>308</v>
       </c>
       <c r="H222" s="11">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="I222" s="11"/>
       <c r="J222" s="7"/>
       <c r="K222" s="11">
         <v>2</v>
       </c>
+      <c r="L222" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M222" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N222" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="O222" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="P222" s="7"/>
+      <c r="Q222" s="7"/>
       <c r="R222" s="7"/>
+    </row>
+    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A223" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C223" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D223" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E223" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F223" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G223" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H223" s="11">
+        <v>2</v>
+      </c>
+      <c r="I223" s="11"/>
+      <c r="J223" s="7"/>
+      <c r="K223" s="11">
+        <v>2</v>
+      </c>
+      <c r="L223" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M223" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N223" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="O223" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="P223" s="7"/>
+      <c r="Q223" s="7"/>
+      <c r="R223" s="7"/>
+    </row>
+    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A224" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="C224" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D224" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E224" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F224" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G224" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H224" s="11">
+        <v>2</v>
+      </c>
+      <c r="I224" s="11"/>
+      <c r="J224" s="7"/>
+      <c r="K224" s="11">
+        <v>2</v>
+      </c>
+      <c r="L224" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M224" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N224" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="O224" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="P224" s="7"/>
+      <c r="Q224" s="7"/>
+      <c r="R224" s="7"/>
+    </row>
+    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A225" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C225" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="D225" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="E225" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F225" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G225" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H225" s="11">
+        <v>2</v>
+      </c>
+      <c r="I225" s="11"/>
+      <c r="J225" s="7"/>
+      <c r="K225" s="11">
+        <v>2</v>
+      </c>
+      <c r="L225" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M225" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N225" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O225" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="P225" s="7"/>
+      <c r="Q225" s="7"/>
+      <c r="R225" s="7"/>
+    </row>
+    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A226" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>618</v>
+      </c>
+      <c r="C226" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="D226" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="E226" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F226" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G226" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H226" s="11">
+        <v>2</v>
+      </c>
+      <c r="I226" s="11"/>
+      <c r="J226" s="7"/>
+      <c r="K226" s="11">
+        <v>2</v>
+      </c>
+      <c r="L226" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M226" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N226" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="O226" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="P226" s="7"/>
+      <c r="Q226" s="7"/>
+      <c r="R226" s="7"/>
+    </row>
+    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A227" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C227" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="D227" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="E227" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F227" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G227" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H227" s="11">
+        <v>2</v>
+      </c>
+      <c r="I227" s="11"/>
+      <c r="J227" s="7"/>
+      <c r="K227" s="11">
+        <v>2</v>
+      </c>
+      <c r="L227" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="M227" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="N227" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="O227" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="P227" s="7"/>
+      <c r="Q227" s="7"/>
+      <c r="R227" s="7"/>
+    </row>
+    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A228" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="B228" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="C228" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="D228" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="E228" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F228" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G228" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H228" s="11">
+        <v>2</v>
+      </c>
+      <c r="I228" s="11"/>
+      <c r="J228" s="7"/>
+      <c r="K228" s="11">
+        <v>2</v>
+      </c>
+      <c r="L228" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M228" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N228" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O228" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P228" s="7"/>
+      <c r="Q228" s="7"/>
+      <c r="R228" s="7"/>
+    </row>
+    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A229" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="B229" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C229" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="D229" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="E229" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F229" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G229" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H229" s="11">
+        <v>2</v>
+      </c>
+      <c r="I229" s="11"/>
+      <c r="J229" s="7"/>
+      <c r="K229" s="11">
+        <v>2</v>
+      </c>
+      <c r="L229" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M229" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N229" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O229" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="P229" s="7"/>
+      <c r="Q229" s="7"/>
+      <c r="R229" s="7"/>
+    </row>
+    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A230" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="B230" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="C230" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="D230" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="E230" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F230" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G230" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H230" s="11">
+        <v>2</v>
+      </c>
+      <c r="I230" s="11"/>
+      <c r="J230" s="7"/>
+      <c r="K230" s="11">
+        <v>2</v>
+      </c>
+      <c r="L230" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M230" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N230" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O230" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="P230" s="7"/>
+      <c r="Q230" s="7"/>
+      <c r="R230" s="7"/>
+    </row>
+    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A231" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="B231" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="C231" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="D231" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="E231" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F231" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G231" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H231" s="11">
+        <v>2</v>
+      </c>
+      <c r="I231" s="11"/>
+      <c r="J231" s="7"/>
+      <c r="K231" s="11">
+        <v>2</v>
+      </c>
+      <c r="L231" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M231" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N231" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O231" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="P231" s="7"/>
+      <c r="Q231" s="7"/>
+      <c r="R231" s="7"/>
+    </row>
+    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A232" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="C232" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="D232" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="E232" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F232" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G232" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H232" s="11">
+        <v>2</v>
+      </c>
+      <c r="I232" s="11"/>
+      <c r="J232" s="7"/>
+      <c r="K232" s="11">
+        <v>2</v>
+      </c>
+      <c r="L232" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M232" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N232" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O232" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="P232" s="7"/>
+      <c r="Q232" s="7"/>
+      <c r="R232" s="7"/>
+    </row>
+    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A233" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="C233" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D233" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E233" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F233" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G233" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H233" s="11">
+        <v>2</v>
+      </c>
+      <c r="I233" s="11"/>
+      <c r="J233" s="7"/>
+      <c r="K233" s="11">
+        <v>2</v>
+      </c>
+      <c r="L233" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M233" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="N233" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="O233" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="P233" s="7"/>
+      <c r="Q233" s="7"/>
+      <c r="R233" s="7"/>
+    </row>
+    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A234" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="C234" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="D234" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="E234" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F234" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G234" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H234" s="11">
+        <v>2</v>
+      </c>
+      <c r="I234" s="11"/>
+      <c r="J234" s="7"/>
+      <c r="K234" s="11">
+        <v>2</v>
+      </c>
+      <c r="L234" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M234" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N234" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O234" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="P234" s="7"/>
+      <c r="Q234" s="7"/>
+      <c r="R234" s="7"/>
+    </row>
+    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A235" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="C235" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D235" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="E235" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F235" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G235" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H235" s="11">
+        <v>2</v>
+      </c>
+      <c r="I235" s="11"/>
+      <c r="J235" s="7"/>
+      <c r="K235" s="11">
+        <v>2</v>
+      </c>
+      <c r="L235" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M235" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="N235" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="O235" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="P235" s="7"/>
+      <c r="Q235" s="7"/>
+      <c r="R235" s="7"/>
+    </row>
+    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A236" s="17" t="s">
+        <v>576</v>
+      </c>
+      <c r="B236" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="C236" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="D236" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="E236" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F236" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G236" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H236" s="11">
+        <v>2</v>
+      </c>
+      <c r="I236" s="11"/>
+      <c r="J236" s="7"/>
+      <c r="K236" s="11">
+        <v>2</v>
+      </c>
+      <c r="L236" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M236" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N236" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="O236" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="P236" s="7"/>
+      <c r="Q236" s="7"/>
+      <c r="R236" s="7"/>
+    </row>
+    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A237" s="17" t="s">
+        <v>577</v>
+      </c>
+      <c r="B237" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="C237" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D237" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E237" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F237" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G237" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H237" s="11">
+        <v>2</v>
+      </c>
+      <c r="I237" s="11"/>
+      <c r="J237" s="7"/>
+      <c r="K237" s="11">
+        <v>2</v>
+      </c>
+      <c r="L237" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M237" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N237" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="O237" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="P237" s="7"/>
+      <c r="Q237" s="7"/>
+      <c r="R237" s="7"/>
+    </row>
+    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A238" s="17" t="s">
+        <v>578</v>
+      </c>
+      <c r="B238" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="C238" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="D238" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="E238" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F238" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G238" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H238" s="11">
+        <v>2</v>
+      </c>
+      <c r="I238" s="11"/>
+      <c r="J238" s="7"/>
+      <c r="K238" s="11">
+        <v>2</v>
+      </c>
+      <c r="L238" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M238" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N238" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O238" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="P238" s="7"/>
+      <c r="Q238" s="7"/>
+      <c r="R238" s="7"/>
+    </row>
+    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A239" s="17" t="s">
+        <v>579</v>
+      </c>
+      <c r="B239" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="C239" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D239" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="E239" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F239" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G239" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H239" s="11">
+        <v>2</v>
+      </c>
+      <c r="I239" s="11"/>
+      <c r="J239" s="7"/>
+      <c r="K239" s="11">
+        <v>2</v>
+      </c>
+      <c r="L239" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M239" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N239" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="O239" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="P239" s="7"/>
+      <c r="Q239" s="7"/>
+      <c r="R239" s="7"/>
+    </row>
+    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A240" s="17" t="s">
+        <v>580</v>
+      </c>
+      <c r="B240" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="C240" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="D240" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="E240" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F240" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G240" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H240" s="11">
+        <v>2</v>
+      </c>
+      <c r="I240" s="11"/>
+      <c r="J240" s="7"/>
+      <c r="K240" s="11">
+        <v>2</v>
+      </c>
+      <c r="L240" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M240" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="N240" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="O240" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="P240" s="7"/>
+      <c r="Q240" s="7"/>
+      <c r="R240" s="7"/>
+    </row>
+    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A241" s="17" t="s">
+        <v>581</v>
+      </c>
+      <c r="B241" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="C241" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="D241" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="E241" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F241" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G241" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H241" s="11">
+        <v>2</v>
+      </c>
+      <c r="I241" s="11"/>
+      <c r="J241" s="7"/>
+      <c r="K241" s="11">
+        <v>2</v>
+      </c>
+      <c r="L241" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M241" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="N241" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="O241" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="P241" s="7"/>
+      <c r="Q241" s="7"/>
+      <c r="R241" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q187">
@@ -13471,4 +15028,65 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF7843F-ECBD-FB43-973C-50114BB7C454}">
+  <dimension ref="A1:R1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>582</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" s="11">
+        <v>2</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="11">
+        <v>2</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>610</v>
+      </c>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>